<commit_message>
Applied HW1 Research Changes to MP and SP
Also removed the SP Kus MS health buff per Echo.
</commit_message>
<xml_diff>
--- a/BalanceInfo/2.3 Harvesting.xlsx
+++ b/BalanceInfo/2.3 Harvesting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Race</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Stats are from Homeworld Remastered as of:</t>
+  </si>
+  <si>
+    <t>Optimally build up to 18 collectors as if it were a real game scenario (build 6 collectors on each ship). Position the mothership at the position three spawn, send carrier to the position three expansion (put 9 collectors on each patch). For vaygr you'll have 19 collectors, one extra on mothership patch.</t>
   </si>
 </sst>
 </file>
@@ -342,14 +345,14 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,7 +771,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -815,24 +818,24 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -1002,24 +1005,24 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
@@ -1257,30 +1260,29 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="18"/>
+      <c r="A42" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="A43" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
@@ -1290,15 +1292,8 @@
         <v>10</v>
       </c>
       <c r="C45" s="20"/>
-      <c r="D45" s="2">
-        <v>28736</v>
-      </c>
-      <c r="E45" s="15">
-        <v>28736</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
@@ -1306,15 +1301,8 @@
         <v>20</v>
       </c>
       <c r="C46" s="22"/>
-      <c r="D46" s="4">
-        <v>74584</v>
-      </c>
-      <c r="E46" s="16">
-        <v>74584</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
@@ -1322,15 +1310,8 @@
         <v>30</v>
       </c>
       <c r="C47" s="22"/>
-      <c r="D47" s="4">
-        <v>120704</v>
-      </c>
-      <c r="E47" s="16">
-        <v>120704</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
@@ -1338,15 +1319,8 @@
         <v>40</v>
       </c>
       <c r="C48" s="24"/>
-      <c r="D48" s="6">
-        <v>166538</v>
-      </c>
-      <c r="E48" s="25">
-        <v>166538</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="25"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
@@ -1356,15 +1330,8 @@
         <v>10</v>
       </c>
       <c r="C49" s="20"/>
-      <c r="D49" s="2">
-        <v>29346</v>
-      </c>
-      <c r="E49" s="3">
-        <v>29360</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
@@ -1372,16 +1339,8 @@
         <v>20</v>
       </c>
       <c r="C50" s="22"/>
-      <c r="D50" s="4">
-        <v>74738</v>
-      </c>
-      <c r="E50" s="5">
-        <v>74862</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="27"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
@@ -1389,15 +1348,8 @@
         <v>30</v>
       </c>
       <c r="C51" s="22"/>
-      <c r="D51" s="4">
-        <v>119750</v>
-      </c>
-      <c r="E51" s="5">
-        <v>120164</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="23"/>
@@ -1405,15 +1357,8 @@
         <v>40</v>
       </c>
       <c r="C52" s="24"/>
-      <c r="D52" s="6">
-        <v>164898</v>
-      </c>
-      <c r="E52" s="31">
-        <v>165276</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>6</v>
-      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
@@ -1423,15 +1368,8 @@
         <v>10</v>
       </c>
       <c r="C53" s="20"/>
-      <c r="D53" s="2">
-        <v>23500</v>
-      </c>
-      <c r="E53" s="3">
-        <v>24000</v>
-      </c>
-      <c r="F53" s="26" t="s">
-        <v>17</v>
-      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
@@ -1439,15 +1377,8 @@
         <v>20</v>
       </c>
       <c r="C54" s="22"/>
-      <c r="D54" s="4">
-        <v>77500</v>
-      </c>
-      <c r="E54" s="5">
-        <v>73800</v>
-      </c>
-      <c r="F54" s="26" t="s">
-        <v>14</v>
-      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
@@ -1455,15 +1386,8 @@
         <v>30</v>
       </c>
       <c r="C55" s="22"/>
-      <c r="D55" s="4">
-        <v>133500</v>
-      </c>
-      <c r="E55" s="5">
-        <v>123300</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>18</v>
-      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="16"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23"/>
@@ -1471,15 +1395,8 @@
         <v>40</v>
       </c>
       <c r="C56" s="24"/>
-      <c r="D56" s="6">
-        <v>187500</v>
-      </c>
-      <c r="E56" s="31">
-        <v>173100</v>
-      </c>
-      <c r="F56" s="26" t="s">
-        <v>5</v>
-      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="25"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
@@ -1490,12 +1407,8 @@
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="3">
-        <v>24000</v>
-      </c>
-      <c r="F57" s="26" t="s">
-        <v>17</v>
-      </c>
+      <c r="E57" s="15"/>
+      <c r="G57" s="26"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
@@ -1504,12 +1417,7 @@
       </c>
       <c r="C58" s="22"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="5">
-        <v>73500</v>
-      </c>
-      <c r="F58" s="26" t="s">
-        <v>14</v>
-      </c>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
@@ -1518,12 +1426,7 @@
       </c>
       <c r="C59" s="22"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="5">
-        <v>124043</v>
-      </c>
-      <c r="F59" s="26" t="s">
-        <v>18</v>
-      </c>
+      <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="23"/>
@@ -1532,18 +1435,306 @@
       </c>
       <c r="C60" s="24"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="31">
+      <c r="E60" s="25"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="31"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="20">
+        <v>10</v>
+      </c>
+      <c r="C65" s="20"/>
+      <c r="D65" s="2">
+        <v>28736</v>
+      </c>
+      <c r="E65" s="15">
+        <v>28736</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="22">
+        <v>20</v>
+      </c>
+      <c r="C66" s="22"/>
+      <c r="D66" s="4">
+        <v>74584</v>
+      </c>
+      <c r="E66" s="16">
+        <v>74584</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="22">
+        <v>30</v>
+      </c>
+      <c r="C67" s="22"/>
+      <c r="D67" s="4">
+        <v>120704</v>
+      </c>
+      <c r="E67" s="16">
+        <v>120704</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="23"/>
+      <c r="B68" s="24">
+        <v>40</v>
+      </c>
+      <c r="C68" s="24"/>
+      <c r="D68" s="6">
+        <v>166538</v>
+      </c>
+      <c r="E68" s="25">
+        <v>166538</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="20">
+        <v>10</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="2">
+        <v>29346</v>
+      </c>
+      <c r="E69" s="3">
+        <v>29360</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="22">
+        <v>20</v>
+      </c>
+      <c r="C70" s="22"/>
+      <c r="D70" s="4">
+        <v>74738</v>
+      </c>
+      <c r="E70" s="5">
+        <v>74862</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="27"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="22">
+        <v>30</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="4">
+        <v>119750</v>
+      </c>
+      <c r="E71" s="5">
+        <v>120164</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="23"/>
+      <c r="B72" s="24">
+        <v>40</v>
+      </c>
+      <c r="C72" s="24"/>
+      <c r="D72" s="6">
+        <v>164898</v>
+      </c>
+      <c r="E72" s="29">
+        <v>165276</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="20">
+        <v>10</v>
+      </c>
+      <c r="C73" s="20"/>
+      <c r="D73" s="2">
+        <v>23500</v>
+      </c>
+      <c r="E73" s="3">
+        <v>24000</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="22">
+        <v>20</v>
+      </c>
+      <c r="C74" s="22"/>
+      <c r="D74" s="4">
+        <v>77500</v>
+      </c>
+      <c r="E74" s="5">
+        <v>73800</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="22">
+        <v>30</v>
+      </c>
+      <c r="C75" s="22"/>
+      <c r="D75" s="4">
+        <v>133500</v>
+      </c>
+      <c r="E75" s="5">
+        <v>123300</v>
+      </c>
+      <c r="F75" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="23"/>
+      <c r="B76" s="24">
+        <v>40</v>
+      </c>
+      <c r="C76" s="24"/>
+      <c r="D76" s="6">
+        <v>187500</v>
+      </c>
+      <c r="E76" s="29">
+        <v>173100</v>
+      </c>
+      <c r="F76" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="20">
+        <v>10</v>
+      </c>
+      <c r="C77" s="20"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="3">
+        <v>24000</v>
+      </c>
+      <c r="F77" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="22">
+        <v>20</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="5">
+        <v>73500</v>
+      </c>
+      <c r="F78" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="22">
+        <v>30</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5">
+        <v>124043</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="23"/>
+      <c r="B80" s="24">
+        <v>40</v>
+      </c>
+      <c r="C80" s="24"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="29">
         <v>174000</v>
       </c>
-      <c r="F60" s="26" t="s">
+      <c r="F80" s="26" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A23:G24"/>
+    <mergeCell ref="A63:G64"/>
+    <mergeCell ref="A3:G4"/>
     <mergeCell ref="A43:G44"/>
-    <mergeCell ref="A3:G4"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>